<commit_message>
Finals documents and pictures
</commit_message>
<xml_diff>
--- a/Lab4/lab4Data.xlsx
+++ b/Lab4/lab4Data.xlsx
@@ -27,32 +27,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Shape</t>
-  </si>
-  <si>
-    <r>
-      <t>Circularity (C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>Centroid</t>
@@ -117,12 +91,40 @@
   <si>
     <t>(812.5827, 592.6496)</t>
   </si>
+  <si>
+    <r>
+      <t>Circularity (C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +133,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -155,16 +166,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,50 +773,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$3:$N$14</c:f>
@@ -2045,22 +2090,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2074,59 +2120,59 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>1.6326000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>19.313400000000001</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="str">
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="str">
         <f>E3</f>
         <v>Rectangle</v>
       </c>
@@ -2164,22 +2210,22 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>15.7722</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="str">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="str">
         <f t="shared" ref="F4:F14" si="0">E4</f>
         <v>Square</v>
       </c>
@@ -2217,22 +2263,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1.0005999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>18.020199999999999</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="str">
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Square</v>
       </c>
@@ -2270,22 +2316,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1.0004999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>13.833399999999999</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="str">
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Circle</v>
       </c>
@@ -2323,23 +2369,23 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>5.4314</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>30.241399999999999</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="H7">
         <f>IF($E7="Rectangle",$B7,NA())</f>
@@ -2375,22 +2421,22 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2.8969999999999998</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>20.802299999999999</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="str">
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Rectangle</v>
       </c>
@@ -2428,22 +2474,22 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1.6738999999999999</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>16.915099999999999</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="str">
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Rectangle</v>
       </c>
@@ -2481,22 +2527,22 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>3.3498000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>22.347000000000001</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="str">
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Ellipses</v>
       </c>
@@ -2534,22 +2580,22 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>2.7170000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>19.485900000000001</v>
       </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" t="str">
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Ellipses</v>
       </c>
@@ -2587,22 +2633,22 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>1.0065</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>13.557700000000001</v>
       </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="str">
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Circle</v>
       </c>
@@ -2640,22 +2686,22 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>1.8601000000000001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>15.981299999999999</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="str">
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Ellipses</v>
       </c>
@@ -2693,22 +2739,22 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>1.7334000000000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>15.4711</v>
       </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="str">
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Ellipses</v>
       </c>

</xml_diff>